<commit_message>
Adding fleshed out calculate class files as well as batch calculate capability for calculate_dIW. Updating other files to cross import as necessary. Also adding a jupyter notebook that will be published with the MEGALab manuscript.
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Python/MetalSilicateFO2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F678A86-979D-574B-BD37-1DEE156A69BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95E9698-5ACB-7B48-8F04-EFE316E5A7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="6960" windowWidth="26840" windowHeight="15940" xr2:uid="{F8D68D9D-4B2A-7140-BC18-AEC977DB5A73}"/>
+    <workbookView xWindow="14260" yWindow="4940" windowWidth="26840" windowHeight="15940" xr2:uid="{F8D68D9D-4B2A-7140-BC18-AEC977DB5A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Label</t>
   </si>
@@ -96,13 +96,7 @@
     <t>ReO3</t>
   </si>
   <si>
-    <t>Cl</t>
-  </si>
-  <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>-O = F + Cl + S</t>
   </si>
   <si>
     <t>Total</t>
@@ -545,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD73AD25-37EC-1D4D-B1F9-86A8E0DC8986}">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,23 +557,21 @@
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,67 +621,58 @@
         <v>19</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AG1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,67 +722,58 @@
         <v>0</v>
       </c>
       <c r="Q2" s="3">
-        <v>1.8307433333333329</v>
-      </c>
-      <c r="R2" s="3">
-        <v>1.9764349999999999</v>
-      </c>
-      <c r="S2" s="3">
-        <v>1.3987983168773179</v>
-      </c>
-      <c r="T2" s="3">
         <v>101.056073516456</v>
       </c>
+      <c r="R2" s="5">
+        <v>6.8510400000000002</v>
+      </c>
+      <c r="S2" s="5">
+        <v>9.8378999999999994E-2</v>
+      </c>
+      <c r="T2" s="5">
+        <v>8.3089999999999997E-2</v>
+      </c>
       <c r="U2" s="5">
-        <v>6.8510400000000002</v>
+        <v>0.47622300000000001</v>
       </c>
       <c r="V2" s="5">
-        <v>9.8378999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="W2" s="5">
-        <v>8.3089999999999997E-2</v>
+        <v>88.444500000000005</v>
       </c>
       <c r="X2" s="5">
-        <v>0.47622300000000001</v>
+        <v>6.6517000000000007E-2</v>
       </c>
       <c r="Y2" s="5">
-        <v>0</v>
+        <v>3.545E-3</v>
       </c>
       <c r="Z2" s="5">
-        <v>88.444500000000005</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="5">
-        <v>6.6517000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="5">
-        <v>3.545E-3</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="5">
         <v>0</v>
       </c>
       <c r="AD2" s="5">
-        <v>0</v>
+        <v>4.9713E-2</v>
       </c>
       <c r="AE2" s="5">
-        <v>0</v>
+        <v>3.1481000000000002E-2</v>
       </c>
       <c r="AF2" s="5">
-        <v>0</v>
+        <v>1.06342</v>
       </c>
       <c r="AG2" s="5">
-        <v>4.9713E-2</v>
-      </c>
-      <c r="AH2" s="5">
-        <v>3.1481000000000002E-2</v>
-      </c>
-      <c r="AI2" s="5">
-        <v>1.06342</v>
-      </c>
-      <c r="AJ2" s="5">
         <v>97.167907999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -849,67 +823,58 @@
         <v>0</v>
       </c>
       <c r="Q3" s="3">
-        <v>1.43</v>
-      </c>
-      <c r="R3" s="3">
-        <v>1.42</v>
-      </c>
-      <c r="S3" s="3">
-        <v>1.0308547526914451</v>
-      </c>
-      <c r="T3" s="3">
         <v>98.949145247308564</v>
       </c>
+      <c r="R3" s="5">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0.17</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.01</v>
+      </c>
       <c r="U3" s="5">
-        <v>19.190000000000001</v>
+        <v>5.53</v>
       </c>
       <c r="V3" s="5">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="W3" s="5">
+        <v>70.7</v>
+      </c>
+      <c r="X3" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="5">
         <v>0.01</v>
       </c>
-      <c r="X3" s="5">
-        <v>5.53</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>70.7</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>1.33</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>0</v>
-      </c>
       <c r="AE3" s="5">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AF3" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AG3" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="AJ3" s="5">
         <v>96.970000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -959,67 +924,58 @@
         <v>0.04</v>
       </c>
       <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="T4" s="3">
         <v>99.1</v>
       </c>
+      <c r="R4" s="5">
+        <v>7.86</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
       <c r="U4" s="5">
-        <v>7.86</v>
+        <v>0.26</v>
       </c>
       <c r="V4" s="5">
-        <v>0</v>
+        <v>3.19</v>
       </c>
       <c r="W4" s="5">
-        <v>0</v>
+        <v>76.34</v>
       </c>
       <c r="X4" s="5">
-        <v>0.26</v>
+        <v>1.17</v>
       </c>
       <c r="Y4" s="5">
-        <v>3.19</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="5">
-        <v>76.34</v>
+        <v>2.6</v>
       </c>
       <c r="AA4" s="5">
-        <v>1.17</v>
+        <v>2.64</v>
       </c>
       <c r="AB4" s="5">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AC4" s="5">
-        <v>2.6</v>
+        <v>1.01</v>
       </c>
       <c r="AD4" s="5">
-        <v>2.64</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="5">
-        <v>4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="5">
-        <v>1.01</v>
+        <v>0.13</v>
       </c>
       <c r="AG4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="AJ4" s="5">
         <v>99.3</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1069,63 +1025,54 @@
         <v>2.4E-2</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="T5" s="3">
         <v>98.897999999999996</v>
       </c>
+      <c r="R5" s="5">
+        <v>1.69</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0</v>
+      </c>
       <c r="U5" s="5">
-        <v>1.69</v>
+        <v>0.15</v>
       </c>
       <c r="V5" s="5">
-        <v>0</v>
+        <v>7.98</v>
       </c>
       <c r="W5" s="5">
-        <v>0</v>
+        <v>80.55</v>
       </c>
       <c r="X5" s="5">
-        <v>0.15</v>
+        <v>0.41</v>
       </c>
       <c r="Y5" s="5">
-        <v>7.98</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="5">
-        <v>80.55</v>
+        <v>2</v>
       </c>
       <c r="AA5" s="5">
-        <v>0.41</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="AB5" s="5">
-        <v>0</v>
+        <v>2.84</v>
       </c>
       <c r="AC5" s="5">
-        <v>2</v>
+        <v>0.06</v>
       </c>
       <c r="AD5" s="5">
-        <v>2.0099999999999998</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="5">
-        <v>2.84</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="5">
-        <v>0.06</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AG5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="5">
-        <v>1.4E-2</v>
-      </c>
-      <c r="AJ5" s="5">
         <v>97.704000000000008</v>
       </c>
     </row>

</xml_diff>